<commit_message>
Added stunning of consonants
</commit_message>
<xml_diff>
--- a/src/data/irregular_exceptions.xlsx
+++ b/src/data/irregular_exceptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RuTranscript\ru_transcript\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB0BC68-8674-4F50-ADFC-C852E9D7DAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB2788E-607D-4B69-8315-39EB55319C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>